<commit_message>
pyPHREEQC master table plotting
Updated pyPHREEQC to pull data from master table, only pulling "vetted"
data
</commit_message>
<xml_diff>
--- a/Sorption Experiments/Sorption Experiment Master Table.xlsx
+++ b/Sorption Experiments/Sorption Experiment Master Table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Dropbox (Personal)\work\MIT Graduate Work\Research\Radium Sorption\Sorption Experiments\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Dropbox (Personal)\work\MIT Graduate Work\Research\RadiumSorption\Sorption Experiments\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="24">
   <si>
     <t>Mineral</t>
   </si>
@@ -57,9 +57,6 @@
   </si>
   <si>
     <t>Ferrihydrite</t>
-  </si>
-  <si>
-    <t>Sample</t>
   </si>
   <si>
     <t>sfSorb</t>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>One sample close to detection</t>
+  </si>
+  <si>
+    <t>Total Activity</t>
   </si>
 </sst>
 </file>
@@ -698,10 +698,10 @@
   <dimension ref="A1:N61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M1" sqref="M1"/>
+      <selection pane="bottomRight" activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -712,7 +712,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -736,7 +736,7 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J1" t="s">
         <v>8</v>
@@ -745,13 +745,13 @@
         <v>3</v>
       </c>
       <c r="L1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="N1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -795,7 +795,7 @@
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -839,7 +839,7 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -883,7 +883,7 @@
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1009,7 +1009,7 @@
         <v>0</v>
       </c>
       <c r="N7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1050,7 +1050,10 @@
         <v>42466</v>
       </c>
       <c r="M8" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="N8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1217,7 +1220,7 @@
         <v>0</v>
       </c>
       <c r="N12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
@@ -1261,7 +1264,7 @@
         <v>1</v>
       </c>
       <c r="N13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
@@ -1510,7 +1513,7 @@
         <v>0</v>
       </c>
       <c r="N19" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -1554,7 +1557,7 @@
         <v>0</v>
       </c>
       <c r="N20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
@@ -1639,7 +1642,7 @@
         <v>0</v>
       </c>
       <c r="N22" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
@@ -1847,7 +1850,7 @@
         <v>0</v>
       </c>
       <c r="N27" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -2055,7 +2058,7 @@
         <v>0</v>
       </c>
       <c r="N32" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -2099,7 +2102,7 @@
         <v>0</v>
       </c>
       <c r="N33" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -2266,7 +2269,7 @@
         <v>0</v>
       </c>
       <c r="N37" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -2310,7 +2313,7 @@
         <v>0</v>
       </c>
       <c r="N38" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
@@ -2441,7 +2444,7 @@
         <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C42">
         <v>0.13246464006479999</v>
@@ -2477,7 +2480,7 @@
         <v>0</v>
       </c>
       <c r="N42" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -2485,7 +2488,7 @@
         <v>50</v>
       </c>
       <c r="B43" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C43">
         <v>0.53340735532888128</v>
@@ -2521,7 +2524,7 @@
         <v>0</v>
       </c>
       <c r="N43" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -2529,7 +2532,7 @@
         <v>100</v>
       </c>
       <c r="B44" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C44">
         <v>1.0549142130593641</v>
@@ -2565,7 +2568,7 @@
         <v>0</v>
       </c>
       <c r="N44" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -2573,7 +2576,7 @@
         <v>250</v>
       </c>
       <c r="B45" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C45">
         <v>2.5786452833352511</v>
@@ -2609,7 +2612,7 @@
         <v>0</v>
       </c>
       <c r="N45" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
@@ -2617,7 +2620,7 @@
         <v>500</v>
       </c>
       <c r="B46" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C46">
         <v>5.163905449696899</v>
@@ -2653,7 +2656,7 @@
         <v>0</v>
       </c>
       <c r="N46" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
@@ -2661,7 +2664,7 @@
         <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C47">
         <v>0.11618094895573838</v>
@@ -2697,7 +2700,7 @@
         <v>0</v>
       </c>
       <c r="N47" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
@@ -2705,7 +2708,7 @@
         <v>50</v>
       </c>
       <c r="B48" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C48">
         <v>0.47181442750076047</v>
@@ -2746,7 +2749,7 @@
         <v>100</v>
       </c>
       <c r="B49" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C49">
         <v>0.9961157116073317</v>
@@ -2787,7 +2790,7 @@
         <v>250</v>
       </c>
       <c r="B50" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C50">
         <v>2.2707584867574684</v>
@@ -2828,7 +2831,7 @@
         <v>500</v>
       </c>
       <c r="B51" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C51">
         <v>4.6275272163134469</v>
@@ -2869,7 +2872,7 @@
         <v>10</v>
       </c>
       <c r="B52" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C52">
         <v>9.3730667323600692E-2</v>
@@ -2910,7 +2913,7 @@
         <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C53">
         <v>0.4088531733731397</v>
@@ -2951,7 +2954,7 @@
         <v>100</v>
       </c>
       <c r="B54" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C54">
         <v>0.8648749751347049</v>
@@ -2992,7 +2995,7 @@
         <v>250</v>
       </c>
       <c r="B55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C55">
         <v>2.0579849634753948</v>
@@ -3033,7 +3036,7 @@
         <v>500</v>
       </c>
       <c r="B56" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C56">
         <v>4.2838693295416412</v>
@@ -3074,7 +3077,7 @@
         <v>10</v>
       </c>
       <c r="B57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C57">
         <v>2.8620228688234051E-2</v>
@@ -3110,7 +3113,7 @@
         <v>0</v>
       </c>
       <c r="N57" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
@@ -3118,7 +3121,7 @@
         <v>50</v>
       </c>
       <c r="B58" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C58">
         <v>5.1055914839843765E-2</v>
@@ -3154,7 +3157,7 @@
         <v>1</v>
       </c>
       <c r="N58" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
@@ -3162,7 +3165,7 @@
         <v>100</v>
       </c>
       <c r="B59" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C59">
         <v>0.11718803711216974</v>
@@ -3203,7 +3206,7 @@
         <v>250</v>
       </c>
       <c r="B60" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C60">
         <v>0.44600961792727273</v>
@@ -3244,7 +3247,7 @@
         <v>500</v>
       </c>
       <c r="B61" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C61">
         <v>0.90169779132976757</v>

</xml_diff>

<commit_message>
Revert "Revert "Added Pyrite, 50 Bq FHY pH9""
This reverts commit 483658a50bd1efab3b0e3584fc7ace352acc108d.
</commit_message>
<xml_diff>
--- a/Sorption Experiments/Sorption Experiment Master Table.xlsx
+++ b/Sorption Experiments/Sorption Experiment Master Table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="26">
   <si>
     <t>Mineral</t>
   </si>
@@ -80,9 +80,6 @@
     <t>Counts close to detection</t>
   </si>
   <si>
-    <t>Need solid counts</t>
-  </si>
-  <si>
     <t>Counts at detection</t>
   </si>
   <si>
@@ -102,6 +99,9 @@
   </si>
   <si>
     <t>Negative Cs, setting to 0</t>
+  </si>
+  <si>
+    <t>Pyrite</t>
   </si>
 </sst>
 </file>
@@ -701,13 +701,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N61"/>
+  <dimension ref="A1:N76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N20" sqref="N20"/>
+      <selection pane="bottomRight" activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -718,7 +718,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -801,7 +801,7 @@
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
@@ -845,7 +845,7 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
@@ -889,7 +889,7 @@
         <v>1</v>
       </c>
       <c r="N4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
@@ -1015,7 +1015,7 @@
         <v>0</v>
       </c>
       <c r="N7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
@@ -1059,7 +1059,7 @@
         <v>0</v>
       </c>
       <c r="N8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
@@ -1486,10 +1486,10 @@
         <v>10</v>
       </c>
       <c r="C19">
-        <v>0</v>
+        <v>0.1106105993106226</v>
       </c>
       <c r="D19">
-        <v>0</v>
+        <v>4.3930737446564849E-3</v>
       </c>
       <c r="E19">
         <v>1665.1142147738785</v>
@@ -1501,10 +1501,10 @@
         <v>49.953426443216358</v>
       </c>
       <c r="H19">
-        <v>1</v>
+        <v>0.77857254809866328</v>
       </c>
       <c r="I19">
-        <v>0</v>
+        <v>8.7943391624000951E-3</v>
       </c>
       <c r="J19">
         <v>8.9166666666666661</v>
@@ -1513,13 +1513,10 @@
         <v>2.5166114784235295E-2</v>
       </c>
       <c r="L19" s="1">
-        <v>42481</v>
+        <v>42507</v>
       </c>
       <c r="M19" t="b">
-        <v>0</v>
-      </c>
-      <c r="N19" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
@@ -1571,31 +1568,31 @@
         <v>10</v>
       </c>
       <c r="C21">
-        <v>4.4084674528744358E-2</v>
+        <v>1.0694639980429503</v>
       </c>
       <c r="D21">
-        <v>2.9860179390728075E-2</v>
+        <v>0.23245961239056712</v>
       </c>
       <c r="E21">
-        <v>13998.532901237906</v>
+        <v>13107.312902868782</v>
       </c>
       <c r="F21">
-        <v>1891.3936416951028</v>
+        <v>774.8653746352262</v>
       </c>
       <c r="G21">
         <v>500.16578689035845</v>
       </c>
       <c r="H21">
-        <v>0.83963357359586033</v>
+        <v>0.78617809812781381</v>
       </c>
       <c r="I21">
-        <v>0.11344600278165595</v>
+        <v>4.6476512085286893E-2</v>
       </c>
       <c r="J21">
-        <v>8.9350000000000005</v>
+        <v>8.913333333333334</v>
       </c>
       <c r="K21">
-        <v>4.7258156262525892E-2</v>
+        <v>2.3094010767584539E-2</v>
       </c>
       <c r="L21" s="1">
         <v>42481</v>
@@ -1853,7 +1850,7 @@
         <v>0</v>
       </c>
       <c r="N27" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
@@ -2061,7 +2058,7 @@
         <v>0</v>
       </c>
       <c r="N32" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
@@ -2272,7 +2269,7 @@
         <v>0</v>
       </c>
       <c r="N37" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -3116,7 +3113,7 @@
         <v>0</v>
       </c>
       <c r="N57" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
@@ -3160,7 +3157,7 @@
         <v>1</v>
       </c>
       <c r="N58" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
@@ -3283,6 +3280,627 @@
         <v>42481</v>
       </c>
       <c r="M61" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>10</v>
+      </c>
+      <c r="B62" t="s">
+        <v>25</v>
+      </c>
+      <c r="C62">
+        <v>0.11242018013969272</v>
+      </c>
+      <c r="D62">
+        <v>7.6718982935510445E-3</v>
+      </c>
+      <c r="E62">
+        <v>-32.109879793362857</v>
+      </c>
+      <c r="F62">
+        <v>22.510987453477643</v>
+      </c>
+      <c r="G62">
+        <v>9.9964568335816697</v>
+      </c>
+      <c r="H62">
+        <v>-0.12460026598657603</v>
+      </c>
+      <c r="I62">
+        <v>7.6746175382645498E-2</v>
+      </c>
+      <c r="J62">
+        <v>2.9933333333333336</v>
+      </c>
+      <c r="K62">
+        <v>1.1547005383792526E-2</v>
+      </c>
+      <c r="L62" s="1">
+        <v>42507</v>
+      </c>
+      <c r="M62" t="b">
+        <v>0</v>
+      </c>
+      <c r="N62" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>50</v>
+      </c>
+      <c r="B63" t="s">
+        <v>25</v>
+      </c>
+      <c r="C63">
+        <v>0.41953747054964391</v>
+      </c>
+      <c r="D63">
+        <v>9.7009736427505835E-3</v>
+      </c>
+      <c r="E63">
+        <v>190.9178399471227</v>
+      </c>
+      <c r="F63">
+        <v>9.482450595268654</v>
+      </c>
+      <c r="G63">
+        <v>50.054201123545624</v>
+      </c>
+      <c r="H63">
+        <v>0.1618336500584116</v>
+      </c>
+      <c r="I63">
+        <v>1.9380937913295773E-2</v>
+      </c>
+      <c r="J63">
+        <v>3.0033333333333334</v>
+      </c>
+      <c r="K63">
+        <v>5.7735026918961348E-3</v>
+      </c>
+      <c r="L63" s="1">
+        <v>42507</v>
+      </c>
+      <c r="M63" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>100</v>
+      </c>
+      <c r="B64" t="s">
+        <v>25</v>
+      </c>
+      <c r="C64">
+        <v>0.833696393431821</v>
+      </c>
+      <c r="D64">
+        <v>1.0256407414719036E-2</v>
+      </c>
+      <c r="E64">
+        <v>420.22702885612733</v>
+      </c>
+      <c r="F64">
+        <v>82.872614278368118</v>
+      </c>
+      <c r="G64">
+        <v>99.964568335816708</v>
+      </c>
+      <c r="H64">
+        <v>0.16600810936217236</v>
+      </c>
+      <c r="I64">
+        <v>1.026004271860013E-2</v>
+      </c>
+      <c r="J64">
+        <v>3.0033333333333334</v>
+      </c>
+      <c r="K64">
+        <v>8.3333333333332742E-3</v>
+      </c>
+      <c r="L64" s="1">
+        <v>42507</v>
+      </c>
+      <c r="M64" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>250</v>
+      </c>
+      <c r="B65" t="s">
+        <v>25</v>
+      </c>
+      <c r="C65">
+        <v>2.0538866741721384</v>
+      </c>
+      <c r="D65">
+        <v>7.088982575508887E-2</v>
+      </c>
+      <c r="E65">
+        <v>1112.8077588728913</v>
+      </c>
+      <c r="F65">
+        <v>323.28915521995827</v>
+      </c>
+      <c r="G65">
+        <v>250.27100561772809</v>
+      </c>
+      <c r="H65">
+        <v>0.17933494968677652</v>
+      </c>
+      <c r="I65">
+        <v>2.8325225121510159E-2</v>
+      </c>
+      <c r="J65">
+        <v>2.9933333333333336</v>
+      </c>
+      <c r="K65">
+        <v>1.1547005383792526E-2</v>
+      </c>
+      <c r="L65" s="1">
+        <v>42507</v>
+      </c>
+      <c r="M65" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>500</v>
+      </c>
+      <c r="B66" t="s">
+        <v>25</v>
+      </c>
+      <c r="C66">
+        <v>4.1755059952216032</v>
+      </c>
+      <c r="D66">
+        <v>1.7745760664004854E-2</v>
+      </c>
+      <c r="E66">
+        <v>2084.8448916576158</v>
+      </c>
+      <c r="F66">
+        <v>332.61036931889845</v>
+      </c>
+      <c r="G66">
+        <v>500.54201123545619</v>
+      </c>
+      <c r="H66">
+        <v>0.16580308915220415</v>
+      </c>
+      <c r="I66">
+        <v>3.5453089382456219E-3</v>
+      </c>
+      <c r="J66">
+        <v>2.9933333333333336</v>
+      </c>
+      <c r="K66">
+        <v>1.1547005383792526E-2</v>
+      </c>
+      <c r="L66" s="1">
+        <v>42507</v>
+      </c>
+      <c r="M66" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>10</v>
+      </c>
+      <c r="B67" t="s">
+        <v>25</v>
+      </c>
+      <c r="C67">
+        <v>0.10124247463533986</v>
+      </c>
+      <c r="D67">
+        <v>3.7540433112101287E-3</v>
+      </c>
+      <c r="E67">
+        <v>-3.4943104645756319E-3</v>
+      </c>
+      <c r="F67">
+        <v>1.0620510693609002E-2</v>
+      </c>
+      <c r="G67">
+        <v>9.9964568335816697</v>
+      </c>
+      <c r="H67">
+        <v>-1.2783592434773757E-2</v>
+      </c>
+      <c r="I67">
+        <v>3.7553739026801571E-2</v>
+      </c>
+      <c r="J67">
+        <v>5.0233333333333334</v>
+      </c>
+      <c r="K67">
+        <v>4.6188021535170098E-2</v>
+      </c>
+      <c r="L67" s="1">
+        <v>42507</v>
+      </c>
+      <c r="M67" t="b">
+        <v>0</v>
+      </c>
+      <c r="N67" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>50</v>
+      </c>
+      <c r="B68" t="s">
+        <v>25</v>
+      </c>
+      <c r="C68">
+        <v>0.41857660141488501</v>
+      </c>
+      <c r="D68">
+        <v>7.2824632120762371E-3</v>
+      </c>
+      <c r="E68">
+        <v>0.22811155763969623</v>
+      </c>
+      <c r="F68">
+        <v>2.5486046404292424E-2</v>
+      </c>
+      <c r="G68">
+        <v>50.054201123545624</v>
+      </c>
+      <c r="H68">
+        <v>0.16375330737626048</v>
+      </c>
+      <c r="I68">
+        <v>1.4549154813401913E-2</v>
+      </c>
+      <c r="J68">
+        <v>4.99</v>
+      </c>
+      <c r="K68">
+        <v>2.6457513110645845E-2</v>
+      </c>
+      <c r="L68" s="1">
+        <v>42507</v>
+      </c>
+      <c r="M68" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>100</v>
+      </c>
+      <c r="B69" t="s">
+        <v>25</v>
+      </c>
+      <c r="C69">
+        <v>0.80130253525997552</v>
+      </c>
+      <c r="D69">
+        <v>5.3444980326268288E-3</v>
+      </c>
+      <c r="E69">
+        <v>0.4851895891200817</v>
+      </c>
+      <c r="F69">
+        <v>8.9480519409142076E-2</v>
+      </c>
+      <c r="G69">
+        <v>99.964568335816708</v>
+      </c>
+      <c r="H69">
+        <v>0.19841344928523677</v>
+      </c>
+      <c r="I69">
+        <v>5.3463923484096433E-3</v>
+      </c>
+      <c r="J69">
+        <v>4.9933333333333332</v>
+      </c>
+      <c r="K69">
+        <v>3.4278273002005234E-2</v>
+      </c>
+      <c r="L69" s="1">
+        <v>42507</v>
+      </c>
+      <c r="M69" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>250</v>
+      </c>
+      <c r="B70" t="s">
+        <v>25</v>
+      </c>
+      <c r="C70">
+        <v>2.001963252193812</v>
+      </c>
+      <c r="D70">
+        <v>3.2713806966716524E-2</v>
+      </c>
+      <c r="E70">
+        <v>1.3872217128592321</v>
+      </c>
+      <c r="F70">
+        <v>0.10820692302913817</v>
+      </c>
+      <c r="G70">
+        <v>250.27100561772809</v>
+      </c>
+      <c r="H70">
+        <v>0.20008182839538591</v>
+      </c>
+      <c r="I70">
+        <v>1.307135314615092E-2</v>
+      </c>
+      <c r="J70">
+        <v>5.0366666666666662</v>
+      </c>
+      <c r="K70">
+        <v>1.5275252316519626E-2</v>
+      </c>
+      <c r="L70" s="1">
+        <v>42507</v>
+      </c>
+      <c r="M70" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>500</v>
+      </c>
+      <c r="B71" t="s">
+        <v>25</v>
+      </c>
+      <c r="C71">
+        <v>3.8313040213701197</v>
+      </c>
+      <c r="D71">
+        <v>2.1103755052666741E-2</v>
+      </c>
+      <c r="E71">
+        <v>2.9951701716397268</v>
+      </c>
+      <c r="F71">
+        <v>0.63458368877856852</v>
+      </c>
+      <c r="G71">
+        <v>500.54201123545619</v>
+      </c>
+      <c r="H71">
+        <v>0.23456894019473931</v>
+      </c>
+      <c r="I71">
+        <v>4.2161805760474614E-3</v>
+      </c>
+      <c r="J71">
+        <v>5.0133333333333328</v>
+      </c>
+      <c r="K71">
+        <v>4.1633319989322265E-2</v>
+      </c>
+      <c r="L71" s="1">
+        <v>42507</v>
+      </c>
+      <c r="M71" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>10</v>
+      </c>
+      <c r="B72" t="s">
+        <v>25</v>
+      </c>
+      <c r="C72">
+        <v>9.5388065223556875E-2</v>
+      </c>
+      <c r="D72">
+        <v>3.7561378736788659E-3</v>
+      </c>
+      <c r="E72">
+        <v>12.043120616528645</v>
+      </c>
+      <c r="F72">
+        <v>10.865681430578073</v>
+      </c>
+      <c r="G72">
+        <v>9.9964568335816697</v>
+      </c>
+      <c r="H72">
+        <v>4.5781252182130312E-2</v>
+      </c>
+      <c r="I72">
+        <v>3.757469207550275E-2</v>
+      </c>
+      <c r="J72">
+        <v>6.9733333333333336</v>
+      </c>
+      <c r="K72">
+        <v>3.2145502536643E-2</v>
+      </c>
+      <c r="L72" s="1">
+        <v>42507</v>
+      </c>
+      <c r="M72" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>50</v>
+      </c>
+      <c r="B73" t="s">
+        <v>25</v>
+      </c>
+      <c r="C73">
+        <v>0.38653546735579836</v>
+      </c>
+      <c r="D73">
+        <v>3.1693400658234991E-3</v>
+      </c>
+      <c r="E73">
+        <v>314.73106445421786</v>
+      </c>
+      <c r="F73">
+        <v>23.973608419002769</v>
+      </c>
+      <c r="G73">
+        <v>50.054201123545624</v>
+      </c>
+      <c r="H73">
+        <v>0.22776618409764002</v>
+      </c>
+      <c r="I73">
+        <v>6.3318163004956254E-3</v>
+      </c>
+      <c r="J73">
+        <v>6.9833333333333334</v>
+      </c>
+      <c r="K73">
+        <v>3.0550504633038766E-2</v>
+      </c>
+      <c r="L73" s="1">
+        <v>42507</v>
+      </c>
+      <c r="M73" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>100</v>
+      </c>
+      <c r="B74" t="s">
+        <v>25</v>
+      </c>
+      <c r="C74">
+        <v>0.75381451764209861</v>
+      </c>
+      <c r="D74">
+        <v>1.3275739434652094E-2</v>
+      </c>
+      <c r="E74">
+        <v>672.4359494534325</v>
+      </c>
+      <c r="F74">
+        <v>100.49085293808112</v>
+      </c>
+      <c r="G74">
+        <v>99.964568335816708</v>
+      </c>
+      <c r="H74">
+        <v>0.24591829866181578</v>
+      </c>
+      <c r="I74">
+        <v>1.3280444917297251E-2</v>
+      </c>
+      <c r="J74">
+        <v>6.9733333333333336</v>
+      </c>
+      <c r="K74">
+        <v>2.5385910352879595E-2</v>
+      </c>
+      <c r="L74" s="1">
+        <v>42507</v>
+      </c>
+      <c r="M74" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>250</v>
+      </c>
+      <c r="B75" t="s">
+        <v>25</v>
+      </c>
+      <c r="C75">
+        <v>1.8424670844240463</v>
+      </c>
+      <c r="D75">
+        <v>9.4925630835149488E-2</v>
+      </c>
+      <c r="E75">
+        <v>1876.8884527803277</v>
+      </c>
+      <c r="F75">
+        <v>497.14252966044381</v>
+      </c>
+      <c r="G75">
+        <v>250.27100561772809</v>
+      </c>
+      <c r="H75">
+        <v>0.263811211420036</v>
+      </c>
+      <c r="I75">
+        <v>3.7929136298010542E-2</v>
+      </c>
+      <c r="J75">
+        <v>7.0166666666666666</v>
+      </c>
+      <c r="K75">
+        <v>2.5166114784235707E-2</v>
+      </c>
+      <c r="L75" s="1">
+        <v>42507</v>
+      </c>
+      <c r="M75" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>500</v>
+      </c>
+      <c r="B76" t="s">
+        <v>25</v>
+      </c>
+      <c r="C76">
+        <v>3.647052296904814</v>
+      </c>
+      <c r="D76">
+        <v>2.8331988697368707E-2</v>
+      </c>
+      <c r="E76">
+        <v>3631.7808435077154</v>
+      </c>
+      <c r="F76">
+        <v>410.3670277910162</v>
+      </c>
+      <c r="G76">
+        <v>500.54201123545619</v>
+      </c>
+      <c r="H76">
+        <v>0.27137938174199899</v>
+      </c>
+      <c r="I76">
+        <v>5.6602618883954767E-3</v>
+      </c>
+      <c r="J76">
+        <v>6.9833333333333334</v>
+      </c>
+      <c r="K76">
+        <v>3.2145502536643007E-2</v>
+      </c>
+      <c r="L76" s="1">
+        <v>42507</v>
+      </c>
+      <c r="M76" t="b">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates to reviewer comments
Also needed to make calculations in the experimental data table to check some assumptions/
</commit_message>
<xml_diff>
--- a/Sorption Experiments/Sorption Experiment Master Table.xlsx
+++ b/Sorption Experiments/Sorption Experiment Master Table.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -1168,10 +1168,10 @@
   <dimension ref="A1:T143"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="P2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomRight" activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>